<commit_message>
modified optimization code, added some comments
</commit_message>
<xml_diff>
--- a/manual_opt_results/results.xlsx
+++ b/manual_opt_results/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajad/PycharmProjects/EORScreeningAPP/saved_model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajad/PycharmProjects/EORScreeningAPP/manual_opt_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFAC103-B419-D748-8D17-5B783F58D403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B645AF-7E9D-B04C-A8A8-2698D26957EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="700" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>train_acc</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>learning_rate</t>
-  </si>
-  <si>
-    <t>pca_enabled</t>
   </si>
 </sst>
 </file>
@@ -431,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,10 +439,10 @@
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -465,19 +462,16 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>32</v>
       </c>
@@ -496,11 +490,8 @@
       <c r="F2">
         <v>200</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>64</v>
       </c>
@@ -519,11 +510,8 @@
       <c r="F3">
         <v>200</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>32</v>
       </c>
@@ -542,11 +530,8 @@
       <c r="F4">
         <v>200</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>32</v>
       </c>
@@ -565,11 +550,8 @@
       <c r="F5">
         <v>200</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>32</v>
       </c>
@@ -588,11 +570,8 @@
       <c r="F6">
         <v>200</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>32</v>
       </c>
@@ -611,11 +590,8 @@
       <c r="F7">
         <v>200</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>32</v>
       </c>
@@ -634,11 +610,8 @@
       <c r="F8">
         <v>200</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>32</v>
       </c>
@@ -657,11 +630,8 @@
       <c r="F9">
         <v>200</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>32</v>
       </c>
@@ -680,11 +650,8 @@
       <c r="F10">
         <v>200</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>32</v>
       </c>
@@ -703,11 +670,8 @@
       <c r="F11">
         <v>200</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>32</v>
       </c>
@@ -726,11 +690,8 @@
       <c r="F12">
         <v>200</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>32</v>
       </c>
@@ -749,11 +710,8 @@
       <c r="F13">
         <v>200</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>32</v>
       </c>
@@ -772,11 +730,8 @@
       <c r="F14">
         <v>200</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>32</v>
       </c>
@@ -795,11 +750,8 @@
       <c r="F15">
         <v>200</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>32</v>
       </c>
@@ -818,11 +770,8 @@
       <c r="F16">
         <v>200</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -841,11 +790,8 @@
       <c r="F17">
         <v>200</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>32</v>
       </c>
@@ -864,11 +810,8 @@
       <c r="F18">
         <v>100</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>32</v>
       </c>
@@ -887,11 +830,8 @@
       <c r="F19">
         <v>300</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>32</v>
       </c>
@@ -910,11 +850,8 @@
       <c r="F20">
         <v>400</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>32</v>
       </c>
@@ -933,11 +870,8 @@
       <c r="F21">
         <v>500</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>32</v>
       </c>
@@ -955,9 +889,6 @@
       </c>
       <c r="F22">
         <v>200</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>